<commit_message>
Pre-deploy: API keys from env, 5/9 deep sources live, GLOPOP-S+WDI integrated
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/cerebro_harm_clock_phase1.xlsx
+++ b/cerebro_harm_clock_phase1.xlsx
@@ -1195,16 +1195,10 @@
       <c r="A4" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="C4" s="9" t="n">
-        <v>59.4</v>
-      </c>
+      <c r="B4" s="9" t="inlineStr"/>
+      <c r="C4" s="9" t="inlineStr"/>
       <c r="D4" s="9" t="inlineStr"/>
-      <c r="E4" s="9" t="n">
-        <v>10.1</v>
-      </c>
+      <c r="E4" s="9" t="inlineStr"/>
       <c r="F4" s="9" t="n">
         <v>5.1</v>
       </c>
@@ -1217,16 +1211,10 @@
       <c r="A5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="C5" s="11" t="n">
-        <v>59.3</v>
-      </c>
+      <c r="B5" s="11" t="inlineStr"/>
+      <c r="C5" s="11" t="inlineStr"/>
       <c r="D5" s="11" t="inlineStr"/>
-      <c r="E5" s="11" t="n">
-        <v>11.3</v>
-      </c>
+      <c r="E5" s="11" t="inlineStr"/>
       <c r="F5" s="11" t="n">
         <v>4.8</v>
       </c>
@@ -1239,16 +1227,10 @@
       <c r="A6" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C6" s="9" t="n">
-        <v>58.8</v>
-      </c>
+      <c r="B6" s="9" t="inlineStr"/>
+      <c r="C6" s="9" t="inlineStr"/>
       <c r="D6" s="9" t="inlineStr"/>
-      <c r="E6" s="9" t="n">
-        <v>11.2</v>
-      </c>
+      <c r="E6" s="9" t="inlineStr"/>
       <c r="F6" s="9" t="n">
         <v>4.6</v>
       </c>
@@ -1261,16 +1243,10 @@
       <c r="A7" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="11" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C7" s="11" t="n">
-        <v>58.7</v>
-      </c>
+      <c r="B7" s="11" t="inlineStr"/>
+      <c r="C7" s="11" t="inlineStr"/>
       <c r="D7" s="11" t="inlineStr"/>
-      <c r="E7" s="11" t="n">
-        <v>10.7</v>
-      </c>
+      <c r="E7" s="11" t="inlineStr"/>
       <c r="F7" s="11" t="n">
         <v>4.6</v>
       </c>
@@ -1283,16 +1259,10 @@
       <c r="A8" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="C8" s="9" t="n">
-        <v>58.7</v>
-      </c>
+      <c r="B8" s="9" t="inlineStr"/>
+      <c r="C8" s="9" t="inlineStr"/>
       <c r="D8" s="9" t="inlineStr"/>
-      <c r="E8" s="9" t="n">
-        <v>11.6</v>
-      </c>
+      <c r="E8" s="9" t="inlineStr"/>
       <c r="F8" s="9" t="n">
         <v>4.9</v>
       </c>
@@ -1305,16 +1275,10 @@
       <c r="A9" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C9" s="11" t="n">
-        <v>58.8</v>
-      </c>
+      <c r="B9" s="11" t="inlineStr"/>
+      <c r="C9" s="11" t="inlineStr"/>
       <c r="D9" s="11" t="inlineStr"/>
-      <c r="E9" s="11" t="n">
-        <v>11.4</v>
-      </c>
+      <c r="E9" s="11" t="inlineStr"/>
       <c r="F9" s="11" t="n">
         <v>5.1</v>
       </c>
@@ -1327,16 +1291,10 @@
       <c r="A10" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="C10" s="9" t="n">
-        <v>59.2</v>
-      </c>
+      <c r="B10" s="9" t="inlineStr"/>
+      <c r="C10" s="9" t="inlineStr"/>
       <c r="D10" s="9" t="inlineStr"/>
-      <c r="E10" s="9" t="n">
-        <v>11.2</v>
-      </c>
+      <c r="E10" s="9" t="inlineStr"/>
       <c r="F10" s="9" t="n">
         <v>5.6</v>
       </c>
@@ -1349,16 +1307,10 @@
       <c r="A11" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="11" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="C11" s="11" t="n">
-        <v>59.6</v>
-      </c>
+      <c r="B11" s="11" t="inlineStr"/>
+      <c r="C11" s="11" t="inlineStr"/>
       <c r="D11" s="11" t="inlineStr"/>
-      <c r="E11" s="11" t="n">
-        <v>12.3</v>
-      </c>
+      <c r="E11" s="11" t="inlineStr"/>
       <c r="F11" s="11" t="n">
         <v>6.2</v>
       </c>
@@ -1371,16 +1323,10 @@
       <c r="A12" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="C12" s="9" t="n">
-        <v>59.6</v>
-      </c>
+      <c r="B12" s="9" t="inlineStr"/>
+      <c r="C12" s="9" t="inlineStr"/>
       <c r="D12" s="9" t="inlineStr"/>
-      <c r="E12" s="9" t="n">
-        <v>11.3</v>
-      </c>
+      <c r="E12" s="9" t="inlineStr"/>
       <c r="F12" s="9" t="n">
         <v>6.9</v>
       </c>
@@ -1395,16 +1341,10 @@
       <c r="A13" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="C13" s="11" t="n">
-        <v>60.1</v>
-      </c>
+      <c r="B13" s="11" t="inlineStr"/>
+      <c r="C13" s="11" t="inlineStr"/>
       <c r="D13" s="11" t="inlineStr"/>
-      <c r="E13" s="11" t="n">
-        <v>10.9</v>
-      </c>
+      <c r="E13" s="11" t="inlineStr"/>
       <c r="F13" s="11" t="n">
         <v>7.3</v>
       </c>
@@ -1419,16 +1359,10 @@
       <c r="A14" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" s="9" t="n">
-        <v>60.4</v>
-      </c>
+      <c r="B14" s="9" t="inlineStr"/>
+      <c r="C14" s="9" t="inlineStr"/>
       <c r="D14" s="9" t="inlineStr"/>
-      <c r="E14" s="9" t="n">
-        <v>12.8</v>
-      </c>
+      <c r="E14" s="9" t="inlineStr"/>
       <c r="F14" s="9" t="n">
         <v>7.9</v>
       </c>
@@ -1443,16 +1377,10 @@
       <c r="A15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B15" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" s="11" t="n">
-        <v>60.2</v>
-      </c>
+      <c r="B15" s="11" t="inlineStr"/>
+      <c r="C15" s="11" t="inlineStr"/>
       <c r="D15" s="11" t="inlineStr"/>
-      <c r="E15" s="11" t="n">
-        <v>13.5</v>
-      </c>
+      <c r="E15" s="11" t="inlineStr"/>
       <c r="F15" s="11" t="n">
         <v>8.6</v>
       </c>
@@ -1467,16 +1395,10 @@
       <c r="A16" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C16" s="9" t="n">
-        <v>60.4</v>
-      </c>
+      <c r="B16" s="9" t="inlineStr"/>
+      <c r="C16" s="9" t="inlineStr"/>
       <c r="D16" s="9" t="inlineStr"/>
-      <c r="E16" s="9" t="n">
-        <v>12.4</v>
-      </c>
+      <c r="E16" s="9" t="inlineStr"/>
       <c r="F16" s="9" t="n">
         <v>9</v>
       </c>
@@ -1491,16 +1413,10 @@
       <c r="A17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B17" s="11" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C17" s="11" t="n">
-        <v>60.8</v>
-      </c>
+      <c r="B17" s="11" t="inlineStr"/>
+      <c r="C17" s="11" t="inlineStr"/>
       <c r="D17" s="11" t="inlineStr"/>
-      <c r="E17" s="11" t="n">
-        <v>13.5</v>
-      </c>
+      <c r="E17" s="11" t="inlineStr"/>
       <c r="F17" s="11" t="n">
         <v>9.4</v>
       </c>
@@ -1515,16 +1431,10 @@
       <c r="A18" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="B18" s="9" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C18" s="9" t="n">
-        <v>61.3</v>
-      </c>
+      <c r="B18" s="9" t="inlineStr"/>
+      <c r="C18" s="9" t="inlineStr"/>
       <c r="D18" s="9" t="inlineStr"/>
-      <c r="E18" s="9" t="n">
-        <v>13.3</v>
-      </c>
+      <c r="E18" s="9" t="inlineStr"/>
       <c r="F18" s="9" t="n">
         <v>9.800000000000001</v>
       </c>
@@ -1539,16 +1449,10 @@
       <c r="A19" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B19" s="11" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="C19" s="11" t="n">
-        <v>61.2</v>
-      </c>
+      <c r="B19" s="11" t="inlineStr"/>
+      <c r="C19" s="11" t="inlineStr"/>
       <c r="D19" s="11" t="inlineStr"/>
-      <c r="E19" s="11" t="n">
-        <v>13.4</v>
-      </c>
+      <c r="E19" s="11" t="inlineStr"/>
       <c r="F19" s="11" t="n">
         <v>9.6</v>
       </c>
@@ -1563,16 +1467,10 @@
       <c r="A20" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="B20" s="9" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <v>61.6</v>
-      </c>
+      <c r="B20" s="9" t="inlineStr"/>
+      <c r="C20" s="9" t="inlineStr"/>
       <c r="D20" s="9" t="inlineStr"/>
-      <c r="E20" s="9" t="n">
-        <v>11.6</v>
-      </c>
+      <c r="E20" s="9" t="inlineStr"/>
       <c r="F20" s="9" t="n">
         <v>8.699999999999999</v>
       </c>
@@ -1587,16 +1485,10 @@
       <c r="A21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="C21" s="11" t="n">
-        <v>62.2</v>
-      </c>
+      <c r="B21" s="11" t="inlineStr"/>
+      <c r="C21" s="11" t="inlineStr"/>
       <c r="D21" s="11" t="inlineStr"/>
-      <c r="E21" s="11" t="n">
-        <v>10.7</v>
-      </c>
+      <c r="E21" s="11" t="inlineStr"/>
       <c r="F21" s="11" t="n">
         <v>8.800000000000001</v>
       </c>
@@ -1611,16 +1503,10 @@
       <c r="A22" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="B22" s="9" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="C22" s="9" t="n">
-        <v>63.2</v>
-      </c>
+      <c r="B22" s="9" t="inlineStr"/>
+      <c r="C22" s="9" t="inlineStr"/>
       <c r="D22" s="9" t="inlineStr"/>
-      <c r="E22" s="9" t="n">
-        <v>10.7</v>
-      </c>
+      <c r="E22" s="9" t="inlineStr"/>
       <c r="F22" s="9" t="n">
         <v>9</v>
       </c>
@@ -1635,16 +1521,10 @@
       <c r="A23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B23" s="11" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C23" s="11" t="n">
-        <v>63.7</v>
-      </c>
+      <c r="B23" s="11" t="inlineStr"/>
+      <c r="C23" s="11" t="inlineStr"/>
       <c r="D23" s="11" t="inlineStr"/>
-      <c r="E23" s="11" t="n">
-        <v>10.3</v>
-      </c>
+      <c r="E23" s="11" t="inlineStr"/>
       <c r="F23" s="11" t="n">
         <v>9.699999999999999</v>
       </c>
@@ -1659,16 +1539,10 @@
       <c r="A24" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="B24" s="9" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="C24" s="9" t="n">
-        <v>63.8</v>
-      </c>
+      <c r="B24" s="9" t="inlineStr"/>
+      <c r="C24" s="9" t="inlineStr"/>
       <c r="D24" s="9" t="inlineStr"/>
-      <c r="E24" s="9" t="n">
-        <v>11.1</v>
-      </c>
+      <c r="E24" s="9" t="inlineStr"/>
       <c r="F24" s="9" t="n">
         <v>10.2</v>
       </c>
@@ -1683,16 +1557,10 @@
       <c r="A25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B25" s="11" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="C25" s="11" t="n">
-        <v>63.9</v>
-      </c>
+      <c r="B25" s="11" t="inlineStr"/>
+      <c r="C25" s="11" t="inlineStr"/>
       <c r="D25" s="11" t="inlineStr"/>
-      <c r="E25" s="11" t="n">
-        <v>11.7</v>
-      </c>
+      <c r="E25" s="11" t="inlineStr"/>
       <c r="F25" s="11" t="n">
         <v>9.800000000000001</v>
       </c>
@@ -1707,16 +1575,10 @@
       <c r="A26" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="B26" s="9" t="n">
-        <v>9.699999999999999</v>
-      </c>
-      <c r="C26" s="9" t="n">
-        <v>64</v>
-      </c>
+      <c r="B26" s="9" t="inlineStr"/>
+      <c r="C26" s="9" t="inlineStr"/>
       <c r="D26" s="9" t="inlineStr"/>
-      <c r="E26" s="9" t="n">
-        <v>12</v>
-      </c>
+      <c r="E26" s="9" t="inlineStr"/>
       <c r="F26" s="9" t="n">
         <v>9.1</v>
       </c>
@@ -1731,16 +1593,10 @@
       <c r="A27" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B27" s="11" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="C27" s="11" t="n">
-        <v>64</v>
-      </c>
+      <c r="B27" s="11" t="inlineStr"/>
+      <c r="C27" s="11" t="inlineStr"/>
       <c r="D27" s="11" t="inlineStr"/>
-      <c r="E27" s="11" t="n">
-        <v>10.1</v>
-      </c>
+      <c r="E27" s="11" t="inlineStr"/>
       <c r="F27" s="11" t="n">
         <v>8.300000000000001</v>
       </c>
@@ -1755,18 +1611,10 @@
       <c r="A28" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="B28" s="9" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="C28" s="9" t="n">
-        <v>64.40000000000001</v>
-      </c>
-      <c r="D28" s="9" t="n">
-        <v>60420</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>11.2</v>
-      </c>
+      <c r="B28" s="9" t="inlineStr"/>
+      <c r="C28" s="9" t="inlineStr"/>
+      <c r="D28" s="9" t="inlineStr"/>
+      <c r="E28" s="9" t="inlineStr"/>
       <c r="F28" s="9" t="n">
         <v>7.9</v>
       </c>
@@ -1781,18 +1629,10 @@
       <c r="A29" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="B29" s="11" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <v>64.8</v>
-      </c>
-      <c r="D29" s="11" t="n">
-        <v>61570</v>
-      </c>
-      <c r="E29" s="11" t="n">
-        <v>9.1</v>
-      </c>
+      <c r="B29" s="11" t="inlineStr"/>
+      <c r="C29" s="11" t="inlineStr"/>
+      <c r="D29" s="11" t="inlineStr"/>
+      <c r="E29" s="11" t="inlineStr"/>
       <c r="F29" s="11" t="n">
         <v>8</v>
       </c>
@@ -1807,18 +1647,10 @@
       <c r="A30" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="B30" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C30" s="9" t="n">
-        <v>65.2</v>
-      </c>
-      <c r="D30" s="9" t="n">
-        <v>63850</v>
-      </c>
-      <c r="E30" s="9" t="n">
-        <v>8.800000000000001</v>
-      </c>
+      <c r="B30" s="9" t="inlineStr"/>
+      <c r="C30" s="9" t="inlineStr"/>
+      <c r="D30" s="9" t="inlineStr"/>
+      <c r="E30" s="9" t="inlineStr"/>
       <c r="F30" s="9" t="n">
         <v>8.6</v>
       </c>
@@ -1833,18 +1665,10 @@
       <c r="A31" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="B31" s="11" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="C31" s="11" t="n">
-        <v>65.59999999999999</v>
-      </c>
-      <c r="D31" s="11" t="n">
-        <v>64650</v>
-      </c>
-      <c r="E31" s="11" t="n">
-        <v>7.5</v>
-      </c>
+      <c r="B31" s="11" t="inlineStr"/>
+      <c r="C31" s="11" t="inlineStr"/>
+      <c r="D31" s="11" t="inlineStr"/>
+      <c r="E31" s="11" t="inlineStr"/>
       <c r="F31" s="11" t="n">
         <v>8.300000000000001</v>
       </c>
@@ -1859,18 +1683,10 @@
       <c r="A32" s="8" t="n">
         <v>28</v>
       </c>
-      <c r="B32" s="9" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="C32" s="9" t="n">
-        <v>65.90000000000001</v>
-      </c>
-      <c r="D32" s="9" t="n">
-        <v>65130</v>
-      </c>
-      <c r="E32" s="9" t="n">
-        <v>8.4</v>
-      </c>
+      <c r="B32" s="9" t="inlineStr"/>
+      <c r="C32" s="9" t="inlineStr"/>
+      <c r="D32" s="9" t="inlineStr"/>
+      <c r="E32" s="9" t="inlineStr"/>
       <c r="F32" s="9" t="n">
         <v>8.5</v>
       </c>
@@ -1885,18 +1701,10 @@
       <c r="A33" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="B33" s="11" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="C33" s="11" t="n">
-        <v>66.40000000000001</v>
-      </c>
-      <c r="D33" s="11" t="n">
-        <v>66240</v>
-      </c>
-      <c r="E33" s="11" t="n">
-        <v>8.300000000000001</v>
-      </c>
+      <c r="B33" s="11" t="inlineStr"/>
+      <c r="C33" s="11" t="inlineStr"/>
+      <c r="D33" s="11" t="inlineStr"/>
+      <c r="E33" s="11" t="inlineStr"/>
       <c r="F33" s="11" t="n">
         <v>8.699999999999999</v>
       </c>
@@ -1911,18 +1719,10 @@
       <c r="A34" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="B34" s="9" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C34" s="9" t="n">
-        <v>66.5</v>
-      </c>
-      <c r="D34" s="9" t="n">
-        <v>65440</v>
-      </c>
-      <c r="E34" s="9" t="n">
-        <v>8.4</v>
-      </c>
+      <c r="B34" s="9" t="inlineStr"/>
+      <c r="C34" s="9" t="inlineStr"/>
+      <c r="D34" s="9" t="inlineStr"/>
+      <c r="E34" s="9" t="inlineStr"/>
       <c r="F34" s="9" t="n">
         <v>9.4</v>
       </c>
@@ -1937,18 +1737,10 @@
       <c r="A35" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="B35" s="11" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="C35" s="11" t="n">
-        <v>66.2</v>
-      </c>
-      <c r="D35" s="11" t="n">
-        <v>63530</v>
-      </c>
-      <c r="E35" s="11" t="n">
-        <v>8.9</v>
-      </c>
+      <c r="B35" s="11" t="inlineStr"/>
+      <c r="C35" s="11" t="inlineStr"/>
+      <c r="D35" s="11" t="inlineStr"/>
+      <c r="E35" s="11" t="inlineStr"/>
       <c r="F35" s="11" t="n">
         <v>9.800000000000001</v>
       </c>
@@ -1963,18 +1755,10 @@
       <c r="A36" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="B36" s="9" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="C36" s="9" t="n">
-        <v>66.40000000000001</v>
-      </c>
-      <c r="D36" s="9" t="n">
-        <v>63010</v>
-      </c>
-      <c r="E36" s="9" t="n">
-        <v>9.4</v>
-      </c>
+      <c r="B36" s="9" t="inlineStr"/>
+      <c r="C36" s="9" t="inlineStr"/>
+      <c r="D36" s="9" t="inlineStr"/>
+      <c r="E36" s="9" t="inlineStr"/>
       <c r="F36" s="9" t="n">
         <v>9.300000000000001</v>
       </c>
@@ -1989,18 +1773,10 @@
       <c r="A37" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="B37" s="11" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="C37" s="11" t="n">
-        <v>66.3</v>
-      </c>
-      <c r="D37" s="11" t="n">
-        <v>62700</v>
-      </c>
-      <c r="E37" s="11" t="n">
-        <v>7.8</v>
-      </c>
+      <c r="B37" s="11" t="inlineStr"/>
+      <c r="C37" s="11" t="inlineStr"/>
+      <c r="D37" s="11" t="inlineStr"/>
+      <c r="E37" s="11" t="inlineStr"/>
       <c r="F37" s="11" t="n">
         <v>9.5</v>
       </c>
@@ -2015,18 +1791,10 @@
       <c r="A38" s="8" t="n">
         <v>34</v>
       </c>
-      <c r="B38" s="9" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="C38" s="9" t="n">
-        <v>66.59999999999999</v>
-      </c>
-      <c r="D38" s="9" t="n">
-        <v>63370</v>
-      </c>
-      <c r="E38" s="9" t="n">
-        <v>6.8</v>
-      </c>
+      <c r="B38" s="9" t="inlineStr"/>
+      <c r="C38" s="9" t="inlineStr"/>
+      <c r="D38" s="9" t="inlineStr"/>
+      <c r="E38" s="9" t="inlineStr"/>
       <c r="F38" s="9" t="n">
         <v>9</v>
       </c>
@@ -2041,18 +1809,10 @@
       <c r="A39" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="B39" s="11" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C39" s="11" t="n">
-        <v>66.59999999999999</v>
-      </c>
-      <c r="D39" s="11" t="n">
-        <v>65380</v>
-      </c>
-      <c r="E39" s="11" t="n">
-        <v>6.9</v>
-      </c>
+      <c r="B39" s="11" t="inlineStr"/>
+      <c r="C39" s="11" t="inlineStr"/>
+      <c r="D39" s="11" t="inlineStr"/>
+      <c r="E39" s="11" t="inlineStr"/>
       <c r="F39" s="11" t="n">
         <v>8.199999999999999</v>
       </c>
@@ -2067,18 +1827,10 @@
       <c r="A40" s="8" t="n">
         <v>36</v>
       </c>
-      <c r="B40" s="9" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C40" s="9" t="n">
-        <v>66.8</v>
-      </c>
-      <c r="D40" s="9" t="n">
-        <v>66340</v>
-      </c>
-      <c r="E40" s="9" t="n">
-        <v>6.3</v>
-      </c>
+      <c r="B40" s="9" t="inlineStr"/>
+      <c r="C40" s="9" t="inlineStr"/>
+      <c r="D40" s="9" t="inlineStr"/>
+      <c r="E40" s="9" t="inlineStr"/>
       <c r="F40" s="9" t="n">
         <v>7.4</v>
       </c>
@@ -2093,18 +1845,10 @@
       <c r="A41" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="B41" s="11" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C41" s="11" t="n">
-        <v>67.09999999999999</v>
-      </c>
-      <c r="D41" s="11" t="n">
-        <v>67720</v>
-      </c>
-      <c r="E41" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="B41" s="11" t="inlineStr"/>
+      <c r="C41" s="11" t="inlineStr"/>
+      <c r="D41" s="11" t="inlineStr"/>
+      <c r="E41" s="11" t="inlineStr"/>
       <c r="F41" s="11" t="n">
         <v>6.8</v>
       </c>
@@ -2119,18 +1863,10 @@
       <c r="A42" s="8" t="n">
         <v>38</v>
       </c>
-      <c r="B42" s="9" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C42" s="9" t="n">
-        <v>67.09999999999999</v>
-      </c>
-      <c r="D42" s="9" t="n">
-        <v>70200</v>
-      </c>
-      <c r="E42" s="9" t="n">
-        <v>6.5</v>
-      </c>
+      <c r="B42" s="9" t="inlineStr"/>
+      <c r="C42" s="9" t="inlineStr"/>
+      <c r="D42" s="9" t="inlineStr"/>
+      <c r="E42" s="9" t="inlineStr"/>
       <c r="F42" s="9" t="n">
         <v>6.3</v>
       </c>
@@ -2145,18 +1881,10 @@
       <c r="A43" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="B43" s="11" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="C43" s="11" t="n">
-        <v>67.09999999999999</v>
-      </c>
-      <c r="D43" s="11" t="n">
-        <v>71980</v>
-      </c>
-      <c r="E43" s="11" t="n">
-        <v>4.6</v>
-      </c>
+      <c r="B43" s="11" t="inlineStr"/>
+      <c r="C43" s="11" t="inlineStr"/>
+      <c r="D43" s="11" t="inlineStr"/>
+      <c r="E43" s="11" t="inlineStr"/>
       <c r="F43" s="11" t="n">
         <v>5.7</v>
       </c>
@@ -2171,18 +1899,10 @@
       <c r="A44" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="B44" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C44" s="9" t="n">
-        <v>67.09999999999999</v>
-      </c>
-      <c r="D44" s="9" t="n">
-        <v>71790</v>
-      </c>
-      <c r="E44" s="9" t="n">
-        <v>4.3</v>
-      </c>
+      <c r="B44" s="9" t="inlineStr"/>
+      <c r="C44" s="9" t="inlineStr"/>
+      <c r="D44" s="9" t="inlineStr"/>
+      <c r="E44" s="9" t="inlineStr"/>
       <c r="F44" s="9" t="n">
         <v>5.5</v>
       </c>
@@ -2197,18 +1917,10 @@
       <c r="A45" s="10" t="n">
         <v>41</v>
       </c>
-      <c r="B45" s="11" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="C45" s="11" t="n">
-        <v>66.8</v>
-      </c>
-      <c r="D45" s="11" t="n">
-        <v>70610</v>
-      </c>
-      <c r="E45" s="11" t="n">
-        <v>4.7</v>
-      </c>
+      <c r="B45" s="11" t="inlineStr"/>
+      <c r="C45" s="11" t="inlineStr"/>
+      <c r="D45" s="11" t="inlineStr"/>
+      <c r="E45" s="11" t="inlineStr"/>
       <c r="F45" s="11" t="n">
         <v>5.6</v>
       </c>
@@ -2223,18 +1935,10 @@
       <c r="A46" s="8" t="n">
         <v>42</v>
       </c>
-      <c r="B46" s="9" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="C46" s="9" t="n">
-        <v>66.59999999999999</v>
-      </c>
-      <c r="D46" s="9" t="n">
-        <v>70040</v>
-      </c>
-      <c r="E46" s="9" t="n">
-        <v>5.6</v>
-      </c>
+      <c r="B46" s="9" t="inlineStr"/>
+      <c r="C46" s="9" t="inlineStr"/>
+      <c r="D46" s="9" t="inlineStr"/>
+      <c r="E46" s="9" t="inlineStr"/>
       <c r="F46" s="9" t="n">
         <v>5.6</v>
       </c>
@@ -2249,18 +1953,10 @@
       <c r="A47" s="10" t="n">
         <v>43</v>
       </c>
-      <c r="B47" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="C47" s="11" t="n">
-        <v>66.2</v>
-      </c>
-      <c r="D47" s="11" t="n">
-        <v>70080</v>
-      </c>
-      <c r="E47" s="11" t="n">
-        <v>5.2</v>
-      </c>
+      <c r="B47" s="11" t="inlineStr"/>
+      <c r="C47" s="11" t="inlineStr"/>
+      <c r="D47" s="11" t="inlineStr"/>
+      <c r="E47" s="11" t="inlineStr"/>
       <c r="F47" s="11" t="n">
         <v>5.7</v>
       </c>
@@ -2275,18 +1971,10 @@
       <c r="A48" s="8" t="n">
         <v>44</v>
       </c>
-      <c r="B48" s="9" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="C48" s="9" t="n">
-        <v>66</v>
-      </c>
-      <c r="D48" s="9" t="n">
-        <v>69970</v>
-      </c>
-      <c r="E48" s="9" t="n">
-        <v>4.7</v>
-      </c>
+      <c r="B48" s="9" t="inlineStr"/>
+      <c r="C48" s="9" t="inlineStr"/>
+      <c r="D48" s="9" t="inlineStr"/>
+      <c r="E48" s="9" t="inlineStr"/>
       <c r="F48" s="9" t="n">
         <v>5.5</v>
       </c>
@@ -2301,18 +1989,10 @@
       <c r="A49" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B49" s="11" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C49" s="11" t="n">
-        <v>66</v>
-      </c>
-      <c r="D49" s="11" t="n">
-        <v>71060</v>
-      </c>
-      <c r="E49" s="11" t="n">
-        <v>2.3</v>
-      </c>
+      <c r="B49" s="11" t="inlineStr"/>
+      <c r="C49" s="11" t="inlineStr"/>
+      <c r="D49" s="11" t="inlineStr"/>
+      <c r="E49" s="11" t="inlineStr"/>
       <c r="F49" s="11" t="n">
         <v>5.6</v>
       </c>
@@ -2327,18 +2007,10 @@
       <c r="A50" s="8" t="n">
         <v>46</v>
       </c>
-      <c r="B50" s="9" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C50" s="9" t="n">
-        <v>66.2</v>
-      </c>
-      <c r="D50" s="9" t="n">
-        <v>71850</v>
-      </c>
-      <c r="E50" s="9" t="n">
-        <v>2.8</v>
-      </c>
+      <c r="B50" s="9" t="inlineStr"/>
+      <c r="C50" s="9" t="inlineStr"/>
+      <c r="D50" s="9" t="inlineStr"/>
+      <c r="E50" s="9" t="inlineStr"/>
       <c r="F50" s="9" t="n">
         <v>5.8</v>
       </c>
@@ -2353,18 +2025,10 @@
       <c r="A51" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B51" s="11" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C51" s="11" t="n">
-        <v>66</v>
-      </c>
-      <c r="D51" s="11" t="n">
-        <v>73010</v>
-      </c>
-      <c r="E51" s="11" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="B51" s="11" t="inlineStr"/>
+      <c r="C51" s="11" t="inlineStr"/>
+      <c r="D51" s="11" t="inlineStr"/>
+      <c r="E51" s="11" t="inlineStr"/>
       <c r="F51" s="11" t="n">
         <v>5.7</v>
       </c>
@@ -2379,18 +2043,10 @@
       <c r="A52" s="8" t="n">
         <v>48</v>
       </c>
-      <c r="B52" s="9" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="C52" s="9" t="n">
-        <v>66</v>
-      </c>
-      <c r="D52" s="9" t="n">
-        <v>70520</v>
-      </c>
-      <c r="E52" s="9" t="n">
-        <v>4.1</v>
-      </c>
+      <c r="B52" s="9" t="inlineStr"/>
+      <c r="C52" s="9" t="inlineStr"/>
+      <c r="D52" s="9" t="inlineStr"/>
+      <c r="E52" s="9" t="inlineStr"/>
       <c r="F52" s="9" t="n">
         <v>5.4</v>
       </c>
@@ -2405,18 +2061,10 @@
       <c r="A53" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="B53" s="11" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="C53" s="11" t="n">
-        <v>65.40000000000001</v>
-      </c>
-      <c r="D53" s="11" t="n">
-        <v>70070</v>
-      </c>
-      <c r="E53" s="11" t="n">
-        <v>5.7</v>
-      </c>
+      <c r="B53" s="11" t="inlineStr"/>
+      <c r="C53" s="11" t="inlineStr"/>
+      <c r="D53" s="11" t="inlineStr"/>
+      <c r="E53" s="11" t="inlineStr"/>
       <c r="F53" s="11" t="n">
         <v>5</v>
       </c>
@@ -2431,18 +2079,10 @@
       <c r="A54" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="B54" s="9" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="C54" s="9" t="n">
-        <v>64.7</v>
-      </c>
-      <c r="D54" s="9" t="n">
-        <v>68420</v>
-      </c>
-      <c r="E54" s="9" t="n">
-        <v>5.9</v>
-      </c>
+      <c r="B54" s="9" t="inlineStr"/>
+      <c r="C54" s="9" t="inlineStr"/>
+      <c r="D54" s="9" t="inlineStr"/>
+      <c r="E54" s="9" t="inlineStr"/>
       <c r="F54" s="9" t="n">
         <v>4.8</v>
       </c>
@@ -2457,18 +2097,10 @@
       <c r="A55" s="10" t="n">
         <v>51</v>
       </c>
-      <c r="B55" s="11" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="C55" s="11" t="n">
-        <v>64.09999999999999</v>
-      </c>
-      <c r="D55" s="11" t="n">
-        <v>67410</v>
-      </c>
-      <c r="E55" s="11" t="n">
-        <v>6.6</v>
-      </c>
+      <c r="B55" s="11" t="inlineStr"/>
+      <c r="C55" s="11" t="inlineStr"/>
+      <c r="D55" s="11" t="inlineStr"/>
+      <c r="E55" s="11" t="inlineStr"/>
       <c r="F55" s="11" t="n">
         <v>4.7</v>
       </c>
@@ -2483,18 +2115,10 @@
       <c r="A56" s="8" t="n">
         <v>52</v>
       </c>
-      <c r="B56" s="9" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="C56" s="9" t="n">
-        <v>63.7</v>
-      </c>
-      <c r="D56" s="9" t="n">
-        <v>67400</v>
-      </c>
-      <c r="E56" s="9" t="n">
-        <v>7.9</v>
-      </c>
+      <c r="B56" s="9" t="inlineStr"/>
+      <c r="C56" s="9" t="inlineStr"/>
+      <c r="D56" s="9" t="inlineStr"/>
+      <c r="E56" s="9" t="inlineStr"/>
       <c r="F56" s="9" t="n">
         <v>4.7</v>
       </c>
@@ -2509,18 +2133,10 @@
       <c r="A57" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="B57" s="11" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="C57" s="11" t="n">
-        <v>63.3</v>
-      </c>
-      <c r="D57" s="11" t="n">
-        <v>69950</v>
-      </c>
-      <c r="E57" s="11" t="n">
-        <v>5</v>
-      </c>
+      <c r="B57" s="11" t="inlineStr"/>
+      <c r="C57" s="11" t="inlineStr"/>
+      <c r="D57" s="11" t="inlineStr"/>
+      <c r="E57" s="11" t="inlineStr"/>
       <c r="F57" s="11" t="n">
         <v>4.5</v>
       </c>
@@ -2535,18 +2151,10 @@
       <c r="A58" s="8" t="n">
         <v>54</v>
       </c>
-      <c r="B58" s="9" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="C58" s="9" t="n">
-        <v>62.9</v>
-      </c>
-      <c r="D58" s="9" t="n">
-        <v>69060</v>
-      </c>
-      <c r="E58" s="9" t="n">
-        <v>5.5</v>
-      </c>
+      <c r="B58" s="9" t="inlineStr"/>
+      <c r="C58" s="9" t="inlineStr"/>
+      <c r="D58" s="9" t="inlineStr"/>
+      <c r="E58" s="9" t="inlineStr"/>
       <c r="F58" s="9" t="n">
         <v>4.4</v>
       </c>
@@ -2561,18 +2169,10 @@
       <c r="A59" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="B59" s="11" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="C59" s="11" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="D59" s="11" t="n">
-        <v>72790</v>
-      </c>
-      <c r="E59" s="11" t="n">
-        <v>5.9</v>
-      </c>
+      <c r="B59" s="11" t="inlineStr"/>
+      <c r="C59" s="11" t="inlineStr"/>
+      <c r="D59" s="11" t="inlineStr"/>
+      <c r="E59" s="11" t="inlineStr"/>
       <c r="F59" s="11" t="n">
         <v>4.9</v>
       </c>
@@ -2587,18 +2187,10 @@
       <c r="A60" s="8" t="n">
         <v>56</v>
       </c>
-      <c r="B60" s="9" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C60" s="9" t="n">
-        <v>62.8</v>
-      </c>
-      <c r="D60" s="9" t="n">
-        <v>75380</v>
-      </c>
-      <c r="E60" s="9" t="n">
-        <v>5.4</v>
-      </c>
+      <c r="B60" s="9" t="inlineStr"/>
+      <c r="C60" s="9" t="inlineStr"/>
+      <c r="D60" s="9" t="inlineStr"/>
+      <c r="E60" s="9" t="inlineStr"/>
       <c r="F60" s="9" t="n">
         <v>5.4</v>
       </c>
@@ -2613,18 +2205,10 @@
       <c r="A61" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="B61" s="11" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C61" s="11" t="n">
-        <v>62.9</v>
-      </c>
-      <c r="D61" s="11" t="n">
-        <v>76710</v>
-      </c>
-      <c r="E61" s="11" t="n">
-        <v>5.8</v>
-      </c>
+      <c r="B61" s="11" t="inlineStr"/>
+      <c r="C61" s="11" t="inlineStr"/>
+      <c r="D61" s="11" t="inlineStr"/>
+      <c r="E61" s="11" t="inlineStr"/>
       <c r="F61" s="11" t="n">
         <v>5.3</v>
       </c>
@@ -2639,18 +2223,10 @@
       <c r="A62" s="8" t="n">
         <v>58</v>
       </c>
-      <c r="B62" s="9" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="C62" s="9" t="n">
-        <v>62.9</v>
-      </c>
-      <c r="D62" s="9" t="n">
-        <v>77700</v>
-      </c>
-      <c r="E62" s="9" t="n">
-        <v>6.4</v>
-      </c>
+      <c r="B62" s="9" t="inlineStr"/>
+      <c r="C62" s="9" t="inlineStr"/>
+      <c r="D62" s="9" t="inlineStr"/>
+      <c r="E62" s="9" t="inlineStr"/>
       <c r="F62" s="9" t="n">
         <v>5</v>
       </c>
@@ -2665,18 +2241,10 @@
       <c r="A63" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="B63" s="11" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="C63" s="11" t="n">
-        <v>63.1</v>
-      </c>
-      <c r="D63" s="11" t="n">
-        <v>83260</v>
-      </c>
-      <c r="E63" s="11" t="n">
-        <v>7.3</v>
-      </c>
+      <c r="B63" s="11" t="inlineStr"/>
+      <c r="C63" s="11" t="inlineStr"/>
+      <c r="D63" s="11" t="inlineStr"/>
+      <c r="E63" s="11" t="inlineStr"/>
       <c r="F63" s="11" t="n">
         <v>5</v>
       </c>
@@ -2691,18 +2259,10 @@
       <c r="A64" s="8" t="n">
         <v>60</v>
       </c>
-      <c r="B64" s="9" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="C64" s="9" t="n">
-        <v>61.7</v>
-      </c>
-      <c r="D64" s="9" t="n">
-        <v>81580</v>
-      </c>
-      <c r="E64" s="9" t="n">
-        <v>15.1</v>
-      </c>
+      <c r="B64" s="9" t="inlineStr"/>
+      <c r="C64" s="9" t="inlineStr"/>
+      <c r="D64" s="9" t="inlineStr"/>
+      <c r="E64" s="9" t="inlineStr"/>
       <c r="F64" s="9" t="n">
         <v>6.5</v>
       </c>
@@ -2717,18 +2277,10 @@
       <c r="A65" s="10" t="n">
         <v>61</v>
       </c>
-      <c r="B65" s="11" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C65" s="11" t="n">
-        <v>61.7</v>
-      </c>
-      <c r="D65" s="11" t="n">
-        <v>81270</v>
-      </c>
-      <c r="E65" s="11" t="n">
-        <v>11.3</v>
-      </c>
+      <c r="B65" s="11" t="inlineStr"/>
+      <c r="C65" s="11" t="inlineStr"/>
+      <c r="D65" s="11" t="inlineStr"/>
+      <c r="E65" s="11" t="inlineStr"/>
       <c r="F65" s="11" t="n">
         <v>6.9</v>
       </c>
@@ -2743,18 +2295,10 @@
       <c r="A66" s="8" t="n">
         <v>62</v>
       </c>
-      <c r="B66" s="9" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="C66" s="9" t="n">
-        <v>62.2</v>
-      </c>
-      <c r="D66" s="9" t="n">
-        <v>79500</v>
-      </c>
-      <c r="E66" s="9" t="n">
-        <v>3.4</v>
-      </c>
+      <c r="B66" s="9" t="inlineStr"/>
+      <c r="C66" s="9" t="inlineStr"/>
+      <c r="D66" s="9" t="inlineStr"/>
+      <c r="E66" s="9" t="inlineStr"/>
       <c r="F66" s="9" t="n">
         <v>6.3</v>
       </c>
@@ -2769,18 +2313,10 @@
       <c r="A67" s="10" t="n">
         <v>63</v>
       </c>
-      <c r="B67" s="11" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="C67" s="11" t="n">
-        <v>62.6</v>
-      </c>
-      <c r="D67" s="11" t="n">
-        <v>82690</v>
-      </c>
-      <c r="E67" s="11" t="n">
-        <v>5.6</v>
-      </c>
+      <c r="B67" s="11" t="inlineStr"/>
+      <c r="C67" s="11" t="inlineStr"/>
+      <c r="D67" s="11" t="inlineStr"/>
+      <c r="E67" s="11" t="inlineStr"/>
       <c r="F67" s="11" t="n">
         <v>5.76</v>
       </c>
@@ -2791,18 +2327,10 @@
       <c r="A68" s="8" t="n">
         <v>64</v>
       </c>
-      <c r="B68" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C68" s="9" t="n">
-        <v>62.6</v>
-      </c>
-      <c r="D68" s="9" t="n">
-        <v>83730</v>
-      </c>
-      <c r="E68" s="9" t="n">
-        <v>5.4</v>
-      </c>
+      <c r="B68" s="9" t="inlineStr"/>
+      <c r="C68" s="9" t="inlineStr"/>
+      <c r="D68" s="9" t="inlineStr"/>
+      <c r="E68" s="9" t="inlineStr"/>
       <c r="F68" s="9" t="inlineStr"/>
       <c r="G68" s="9" t="inlineStr"/>
       <c r="H68" s="9" t="inlineStr"/>
@@ -3928,7 +3456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4004,13 +3532,13 @@
         <v>1979</v>
       </c>
       <c r="C5" s="18" t="n">
-        <v>0.86</v>
+        <v>2.83</v>
       </c>
       <c r="D5" s="18" t="n">
-        <v>-0.009900000000000001</v>
+        <v>-0.0355</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>0.0417</v>
+        <v>0.0287</v>
       </c>
       <c r="F5" s="18" t="n">
         <v>2</v>
@@ -4028,16 +3556,16 @@
     </row>
     <row r="6" ht="28" customHeight="1">
       <c r="B6" s="17" t="n">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="C6" s="18" t="n">
-        <v>-0.59</v>
+        <v>3.04</v>
       </c>
       <c r="D6" s="18" t="n">
-        <v>-0.0455</v>
+        <v>-0.0405</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.0098</v>
       </c>
       <c r="F6" s="18" t="n">
         <v>2</v>
@@ -4054,44 +3582,44 @@
       </c>
     </row>
     <row r="7" ht="28" customHeight="1">
-      <c r="B7" s="21" t="n">
-        <v>1995</v>
-      </c>
-      <c r="C7" s="22" t="n">
-        <v>-1.72</v>
-      </c>
-      <c r="D7" s="22" t="n">
-        <v>-0.0022</v>
-      </c>
-      <c r="E7" s="22" t="n">
-        <v>0.0321</v>
-      </c>
-      <c r="F7" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="23" t="inlineStr">
-        <is>
-          <t>STRONG SADDLE ⚡</t>
-        </is>
-      </c>
-      <c r="H7" s="24" t="inlineStr">
-        <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+      <c r="B7" s="17" t="n">
+        <v>1982</v>
+      </c>
+      <c r="C7" s="18" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>-0.022</v>
+      </c>
+      <c r="E7" s="18" t="n">
+        <v>0.0201</v>
+      </c>
+      <c r="F7" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H7" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="8" ht="28" customHeight="1">
       <c r="B8" s="17" t="n">
-        <v>1996</v>
+        <v>1985</v>
       </c>
       <c r="C8" s="18" t="n">
-        <v>0.12</v>
+        <v>3.04</v>
       </c>
       <c r="D8" s="18" t="n">
-        <v>0.0433</v>
+        <v>-0.0001</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0.0335</v>
+        <v>0.0135</v>
       </c>
       <c r="F8" s="18" t="n">
         <v>2</v>
@@ -4109,16 +3637,16 @@
     </row>
     <row r="9" ht="28" customHeight="1">
       <c r="B9" s="17" t="n">
-        <v>1997</v>
+        <v>1986</v>
       </c>
       <c r="C9" s="18" t="n">
-        <v>-0.59</v>
+        <v>2.48</v>
       </c>
       <c r="D9" s="18" t="n">
-        <v>0.0221</v>
+        <v>-0.0024</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>0.0224</v>
+        <v>0.0065</v>
       </c>
       <c r="F9" s="18" t="n">
         <v>2</v>
@@ -4135,125 +3663,125 @@
       </c>
     </row>
     <row r="10" ht="28" customHeight="1">
-      <c r="B10" s="17" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C10" s="18" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="D10" s="18" t="n">
-        <v>0.0912</v>
-      </c>
-      <c r="E10" s="18" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="F10" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H10" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+      <c r="B10" s="21" t="n">
+        <v>1993</v>
+      </c>
+      <c r="C10" s="22" t="n">
+        <v>-2.22</v>
+      </c>
+      <c r="D10" s="22" t="n">
+        <v>-0.0575</v>
+      </c>
+      <c r="E10" s="22" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="F10" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" s="23" t="inlineStr">
+        <is>
+          <t>STRONG SADDLE ⚡</t>
+        </is>
+      </c>
+      <c r="H10" s="24" t="inlineStr">
+        <is>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
         </is>
       </c>
     </row>
     <row r="11" ht="28" customHeight="1">
-      <c r="B11" s="17" t="n">
-        <v>2002</v>
-      </c>
-      <c r="C11" s="18" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="D11" s="18" t="n">
-        <v>0.0301</v>
-      </c>
-      <c r="E11" s="18" t="n">
-        <v>0.0066</v>
-      </c>
-      <c r="F11" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H11" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+      <c r="B11" s="21" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C11" s="22" t="n">
+        <v>-3.36</v>
+      </c>
+      <c r="D11" s="22" t="n">
+        <v>-0.0491</v>
+      </c>
+      <c r="E11" s="22" t="n">
+        <v>0.0102</v>
+      </c>
+      <c r="F11" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="23" t="inlineStr">
+        <is>
+          <t>STRONG SADDLE ⚡</t>
+        </is>
+      </c>
+      <c r="H11" s="24" t="inlineStr">
+        <is>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
         </is>
       </c>
     </row>
     <row r="12" ht="28" customHeight="1">
-      <c r="B12" s="17" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C12" s="18" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="D12" s="18" t="n">
-        <v>0.0689</v>
-      </c>
-      <c r="E12" s="18" t="n">
-        <v>0.0544</v>
-      </c>
-      <c r="F12" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H12" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+      <c r="B12" s="21" t="n">
+        <v>1996</v>
+      </c>
+      <c r="C12" s="22" t="n">
+        <v>-2.23</v>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="E12" s="22" t="n">
+        <v>0.0191</v>
+      </c>
+      <c r="F12" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="23" t="inlineStr">
+        <is>
+          <t>STRONG SADDLE ⚡</t>
+        </is>
+      </c>
+      <c r="H12" s="24" t="inlineStr">
+        <is>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
         </is>
       </c>
     </row>
     <row r="13" ht="28" customHeight="1">
-      <c r="B13" s="17" t="n">
-        <v>2008</v>
-      </c>
-      <c r="C13" s="18" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D13" s="18" t="n">
-        <v>0.0622</v>
-      </c>
-      <c r="E13" s="18" t="n">
-        <v>0.0468</v>
-      </c>
-      <c r="F13" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H13" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+      <c r="B13" s="21" t="n">
+        <v>1997</v>
+      </c>
+      <c r="C13" s="22" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="D13" s="22" t="n">
+        <v>-0.0041</v>
+      </c>
+      <c r="E13" s="22" t="n">
+        <v>0.0221</v>
+      </c>
+      <c r="F13" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="23" t="inlineStr">
+        <is>
+          <t>STRONG SADDLE ⚡</t>
+        </is>
+      </c>
+      <c r="H13" s="24" t="inlineStr">
+        <is>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
         </is>
       </c>
     </row>
     <row r="14" ht="28" customHeight="1">
       <c r="B14" s="17" t="n">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="C14" s="18" t="n">
-        <v>-0.9</v>
+        <v>-1.49</v>
       </c>
       <c r="D14" s="18" t="n">
-        <v>0.0168</v>
+        <v>0.0494</v>
       </c>
       <c r="E14" s="18" t="n">
-        <v>0.0367</v>
+        <v>0.0179</v>
       </c>
       <c r="F14" s="18" t="n">
         <v>2</v>
@@ -4271,16 +3799,16 @@
     </row>
     <row r="15" ht="28" customHeight="1">
       <c r="B15" s="17" t="n">
-        <v>2012</v>
+        <v>2002</v>
       </c>
       <c r="C15" s="18" t="n">
-        <v>-0.31</v>
+        <v>-1.54</v>
       </c>
       <c r="D15" s="18" t="n">
-        <v>0.1267</v>
+        <v>0.0351</v>
       </c>
       <c r="E15" s="18" t="n">
-        <v>0.1032</v>
+        <v>0.0158</v>
       </c>
       <c r="F15" s="18" t="n">
         <v>2</v>
@@ -4298,16 +3826,16 @@
     </row>
     <row r="16" ht="28" customHeight="1">
       <c r="B16" s="17" t="n">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="C16" s="18" t="n">
-        <v>0.6</v>
+        <v>-2.42</v>
       </c>
       <c r="D16" s="18" t="n">
-        <v>0.171</v>
+        <v>0.0164</v>
       </c>
       <c r="E16" s="18" t="n">
-        <v>0.1167</v>
+        <v>0.0213</v>
       </c>
       <c r="F16" s="18" t="n">
         <v>2</v>
@@ -4325,16 +3853,16 @@
     </row>
     <row r="17" ht="28" customHeight="1">
       <c r="B17" s="17" t="n">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="C17" s="18" t="n">
-        <v>0.85</v>
+        <v>-2.35</v>
       </c>
       <c r="D17" s="18" t="n">
-        <v>0.147</v>
+        <v>0.0392</v>
       </c>
       <c r="E17" s="18" t="n">
-        <v>0.0785</v>
+        <v>0.0352</v>
       </c>
       <c r="F17" s="18" t="n">
         <v>2</v>
@@ -4352,16 +3880,16 @@
     </row>
     <row r="18" ht="28" customHeight="1">
       <c r="B18" s="17" t="n">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="C18" s="18" t="n">
-        <v>1.8</v>
+        <v>-1.98</v>
       </c>
       <c r="D18" s="18" t="n">
-        <v>0.171</v>
+        <v>0.0774</v>
       </c>
       <c r="E18" s="18" t="n">
-        <v>0.0906</v>
+        <v>0.0551</v>
       </c>
       <c r="F18" s="18" t="n">
         <v>2</v>
@@ -4378,44 +3906,44 @@
       </c>
     </row>
     <row r="19" ht="28" customHeight="1">
-      <c r="B19" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="C19" s="22" t="n">
-        <v>-4.37</v>
-      </c>
-      <c r="D19" s="22" t="n">
-        <v>-0.0437</v>
-      </c>
-      <c r="E19" s="22" t="n">
-        <v>0.0261</v>
-      </c>
-      <c r="F19" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="G19" s="23" t="inlineStr">
-        <is>
-          <t>STRONG SADDLE ⚡</t>
-        </is>
-      </c>
-      <c r="H19" s="24" t="inlineStr">
-        <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+      <c r="B19" s="17" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C19" s="18" t="n">
+        <v>-1.52</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>0.0963</v>
+      </c>
+      <c r="E19" s="18" t="n">
+        <v>0.0542</v>
+      </c>
+      <c r="F19" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H19" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="20" ht="28" customHeight="1">
       <c r="B20" s="17" t="n">
-        <v>2022</v>
+        <v>2014</v>
       </c>
       <c r="C20" s="18" t="n">
-        <v>0.77</v>
+        <v>-1.15</v>
       </c>
       <c r="D20" s="18" t="n">
-        <v>0.1107</v>
+        <v>0.107</v>
       </c>
       <c r="E20" s="18" t="n">
-        <v>0.0746</v>
+        <v>0.0579</v>
       </c>
       <c r="F20" s="18" t="n">
         <v>2</v>
@@ -4426,6 +3954,114 @@
         </is>
       </c>
       <c r="H20" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="28" customHeight="1">
+      <c r="B21" s="17" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="18" t="n">
+        <v>-1.69</v>
+      </c>
+      <c r="D21" s="18" t="n">
+        <v>0.0683</v>
+      </c>
+      <c r="E21" s="18" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="F21" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H21" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="28" customHeight="1">
+      <c r="B22" s="17" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="18" t="n">
+        <v>0.1026</v>
+      </c>
+      <c r="E22" s="18" t="n">
+        <v>0.06270000000000001</v>
+      </c>
+      <c r="F22" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H22" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="28" customHeight="1">
+      <c r="B23" s="17" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="18" t="n">
+        <v>-3.49</v>
+      </c>
+      <c r="D23" s="18" t="n">
+        <v>0.0304</v>
+      </c>
+      <c r="E23" s="18" t="n">
+        <v>0.0463</v>
+      </c>
+      <c r="F23" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H23" s="20" t="inlineStr">
+        <is>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="28" customHeight="1">
+      <c r="B24" s="17" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C24" s="18" t="n">
+        <v>-1.56</v>
+      </c>
+      <c r="D24" s="18" t="n">
+        <v>0.07729999999999999</v>
+      </c>
+      <c r="E24" s="18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="19" t="inlineStr">
+        <is>
+          <t>MODERATE SADDLE</t>
+        </is>
+      </c>
+      <c r="H24" s="20" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
@@ -4481,13 +4117,13 @@
         <v>1979</v>
       </c>
       <c r="B2" t="n">
-        <v>0.857</v>
+        <v>2.83</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.009900000000000001</v>
+        <v>-0.0355</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0417</v>
+        <v>0.0287</v>
       </c>
     </row>
     <row r="3">
@@ -4495,13 +4131,13 @@
         <v>1980</v>
       </c>
       <c r="B3" t="n">
-        <v>1.049</v>
+        <v>3.041</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0111</v>
+        <v>-0.0405</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0365</v>
+        <v>0.0098</v>
       </c>
     </row>
     <row r="4">
@@ -4509,13 +4145,13 @@
         <v>1982</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.587</v>
+        <v>2.55</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0455</v>
+        <v>-0.022</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.0201</v>
       </c>
     </row>
     <row r="5">
@@ -4523,13 +4159,13 @@
         <v>1984</v>
       </c>
       <c r="B5" t="n">
-        <v>1.814</v>
+        <v>3.571</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0319</v>
+        <v>0.0247</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0139</v>
+        <v>0.0201</v>
       </c>
     </row>
     <row r="6">
@@ -4537,13 +4173,13 @@
         <v>1985</v>
       </c>
       <c r="B6" t="n">
-        <v>1.647</v>
+        <v>3.037</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0199</v>
+        <v>-0.0001</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0029</v>
+        <v>0.0135</v>
       </c>
     </row>
     <row r="7">
@@ -4551,13 +4187,13 @@
         <v>1986</v>
       </c>
       <c r="B7" t="n">
-        <v>1.675</v>
+        <v>2.477</v>
       </c>
       <c r="C7" t="n">
-        <v>0.07539999999999999</v>
+        <v>-0.0024</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0403</v>
+        <v>0.0065</v>
       </c>
     </row>
     <row r="8">
@@ -4565,13 +4201,13 @@
         <v>1987</v>
       </c>
       <c r="B8" t="n">
-        <v>2.025</v>
+        <v>2.266</v>
       </c>
       <c r="C8" t="n">
-        <v>0.007</v>
+        <v>-0.0435</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0083</v>
+        <v>-0.0227</v>
       </c>
     </row>
     <row r="9">
@@ -4579,13 +4215,13 @@
         <v>1988</v>
       </c>
       <c r="B9" t="n">
-        <v>1.409</v>
+        <v>1.269</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.007900000000000001</v>
+        <v>-0.0589</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.009299999999999999</v>
+        <v>-0.0196</v>
       </c>
     </row>
     <row r="10">
@@ -4593,13 +4229,13 @@
         <v>1989</v>
       </c>
       <c r="B10" t="n">
-        <v>1.294</v>
+        <v>0.503</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0127</v>
+        <v>-0.0658</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0294</v>
+        <v>-0.0211</v>
       </c>
     </row>
     <row r="11">
@@ -4607,13 +4243,13 @@
         <v>1990</v>
       </c>
       <c r="B11" t="n">
-        <v>0.541</v>
+        <v>-0.491</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0494</v>
+        <v>-0.0919</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0188</v>
+        <v>-0.0161</v>
       </c>
     </row>
     <row r="12">
@@ -4621,13 +4257,13 @@
         <v>1991</v>
       </c>
       <c r="B12" t="n">
-        <v>0.096</v>
+        <v>-0.737</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0438</v>
+        <v>-0.0669</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0119</v>
+        <v>-0.0026</v>
       </c>
     </row>
     <row r="13">
@@ -4635,13 +4271,13 @@
         <v>1992</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.656</v>
+        <v>-1.89</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0983</v>
+        <v>-0.0798</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.0285</v>
+        <v>-0.0047</v>
       </c>
     </row>
     <row r="14">
@@ -4649,13 +4285,13 @@
         <v>1993</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.178</v>
+        <v>-2.216</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0573</v>
+        <v>-0.0575</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0026</v>
+        <v>0.0115</v>
       </c>
     </row>
     <row r="15">
@@ -4663,13 +4299,13 @@
         <v>1994</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.254</v>
+        <v>-2.846</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.045</v>
+        <v>-0.0703</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0004</v>
+        <v>-0.0011</v>
       </c>
     </row>
     <row r="16">
@@ -4677,13 +4313,13 @@
         <v>1995</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.721</v>
+        <v>-3.363</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0022</v>
+        <v>-0.0491</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0321</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="17">
@@ -4691,13 +4327,13 @@
         <v>1996</v>
       </c>
       <c r="B17" t="n">
-        <v>0.122</v>
+        <v>-2.226</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0433</v>
+        <v>-0.0003</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0335</v>
+        <v>0.0191</v>
       </c>
     </row>
     <row r="18">
@@ -4705,13 +4341,13 @@
         <v>1997</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.591</v>
+        <v>-2.97</v>
       </c>
       <c r="C18" t="n">
+        <v>-0.0041</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.0221</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.0224</v>
       </c>
     </row>
     <row r="19">
@@ -4719,13 +4355,13 @@
         <v>1998</v>
       </c>
       <c r="B19" t="n">
-        <v>1.279</v>
+        <v>-1.915</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1</v>
+        <v>0.0483</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0341</v>
+        <v>0.0325</v>
       </c>
     </row>
     <row r="20">
@@ -4733,13 +4369,13 @@
         <v>1999</v>
       </c>
       <c r="B20" t="n">
-        <v>0.428</v>
+        <v>-2.594</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0102</v>
+        <v>-0.0123</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.011</v>
+        <v>-0.004</v>
       </c>
     </row>
     <row r="21">
@@ -4747,13 +4383,13 @@
         <v>2000</v>
       </c>
       <c r="B21" t="n">
-        <v>2.146</v>
+        <v>-1.486</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0912</v>
+        <v>0.0494</v>
       </c>
       <c r="D21" t="n">
-        <v>0.023</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="22">
@@ -4761,13 +4397,13 @@
         <v>2001</v>
       </c>
       <c r="B22" t="n">
-        <v>1.662</v>
+        <v>-1.498</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0128</v>
+        <v>0.0139</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0291</v>
+        <v>-0.0115</v>
       </c>
     </row>
     <row r="23">
@@ -4775,13 +4411,13 @@
         <v>2002</v>
       </c>
       <c r="B23" t="n">
-        <v>1.332</v>
+        <v>-1.542</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0301</v>
+        <v>0.0351</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0066</v>
+        <v>0.0158</v>
       </c>
     </row>
     <row r="24">
@@ -4789,13 +4425,13 @@
         <v>2003</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.6879999999999999</v>
+        <v>-2.91</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.0945</v>
+        <v>-0.0475</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0619</v>
+        <v>-0.0323</v>
       </c>
     </row>
     <row r="25">
@@ -4803,13 +4439,13 @@
         <v>2004</v>
       </c>
       <c r="B25" t="n">
-        <v>1.387</v>
+        <v>-1.66</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.0092</v>
+        <v>-0.0054</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.0073</v>
+        <v>-0.0064</v>
       </c>
     </row>
     <row r="26">
@@ -4817,13 +4453,13 @@
         <v>2005</v>
       </c>
       <c r="B26" t="n">
-        <v>-1.016</v>
+        <v>-3.53</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.07820000000000001</v>
+        <v>-0.0663</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.0361</v>
+        <v>-0.0338</v>
       </c>
     </row>
     <row r="27">
@@ -4831,13 +4467,13 @@
         <v>2006</v>
       </c>
       <c r="B27" t="n">
-        <v>1.378</v>
+        <v>-2.417</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0689</v>
+        <v>0.0164</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0544</v>
+        <v>0.0213</v>
       </c>
     </row>
     <row r="28">
@@ -4845,13 +4481,13 @@
         <v>2007</v>
       </c>
       <c r="B28" t="n">
-        <v>-1.409</v>
+        <v>-4.3</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.09320000000000001</v>
+        <v>-0.08799999999999999</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.028</v>
+        <v>-0.0275</v>
       </c>
     </row>
     <row r="29">
@@ -4859,13 +4495,13 @@
         <v>2008</v>
       </c>
       <c r="B29" t="n">
-        <v>0.851</v>
+        <v>-2.354</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0622</v>
+        <v>0.0392</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0468</v>
+        <v>0.0352</v>
       </c>
     </row>
     <row r="30">
@@ -4873,13 +4509,13 @@
         <v>2009</v>
       </c>
       <c r="B30" t="n">
-        <v>-4.112</v>
+        <v>-4.403</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.183</v>
+        <v>-0.06619999999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0839</v>
+        <v>-0.0275</v>
       </c>
     </row>
     <row r="31">
@@ -4887,13 +4523,13 @@
         <v>2010</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.904</v>
+        <v>-1.977</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0168</v>
+        <v>0.0774</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0367</v>
+        <v>0.0551</v>
       </c>
     </row>
     <row r="32">
@@ -4901,13 +4537,13 @@
         <v>2011</v>
       </c>
       <c r="B32" t="n">
-        <v>-4.527</v>
+        <v>-4.356</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.1793</v>
+        <v>-0.0667</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0805</v>
+        <v>-0.0353</v>
       </c>
     </row>
     <row r="33">
@@ -4915,13 +4551,13 @@
         <v>2012</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.31</v>
+        <v>-1.515</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1267</v>
+        <v>0.0963</v>
       </c>
       <c r="D33" t="n">
-        <v>0.1032</v>
+        <v>0.0542</v>
       </c>
     </row>
     <row r="34">
@@ -4929,13 +4565,13 @@
         <v>2013</v>
       </c>
       <c r="B34" t="n">
-        <v>-3.561</v>
+        <v>-3.745</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.0886</v>
+        <v>-0.0589</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0351</v>
+        <v>-0.0455</v>
       </c>
     </row>
     <row r="35">
@@ -4943,13 +4579,13 @@
         <v>2014</v>
       </c>
       <c r="B35" t="n">
-        <v>0.602</v>
+        <v>-1.148</v>
       </c>
       <c r="C35" t="n">
-        <v>0.171</v>
+        <v>0.107</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1167</v>
+        <v>0.0579</v>
       </c>
     </row>
     <row r="36">
@@ -4957,13 +4593,13 @@
         <v>2015</v>
       </c>
       <c r="B36" t="n">
-        <v>-3.334</v>
+        <v>-4.083</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.1008</v>
+        <v>-0.0856</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.07580000000000001</v>
+        <v>-0.0606</v>
       </c>
     </row>
     <row r="37">
@@ -4971,13 +4607,13 @@
         <v>2016</v>
       </c>
       <c r="B37" t="n">
-        <v>0.848</v>
+        <v>-1.695</v>
       </c>
       <c r="C37" t="n">
-        <v>0.147</v>
+        <v>0.0683</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0785</v>
+        <v>0.0424</v>
       </c>
     </row>
     <row r="38">
@@ -4985,13 +4621,13 @@
         <v>2017</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.057</v>
+        <v>-4.401</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.122</v>
+        <v>-0.1084</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.09760000000000001</v>
+        <v>-0.0718</v>
       </c>
     </row>
     <row r="39">
@@ -4999,13 +4635,13 @@
         <v>2018</v>
       </c>
       <c r="B39" t="n">
-        <v>1.797</v>
+        <v>-1.005</v>
       </c>
       <c r="C39" t="n">
-        <v>0.171</v>
+        <v>0.1026</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0906</v>
+        <v>0.06270000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -5013,13 +4649,13 @@
         <v>2019</v>
       </c>
       <c r="B40" t="n">
-        <v>-2.545</v>
+        <v>-3.877</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.1131</v>
+        <v>-0.0727</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.0867</v>
+        <v>-0.047</v>
       </c>
     </row>
     <row r="41">
@@ -5027,13 +4663,13 @@
         <v>2020</v>
       </c>
       <c r="B41" t="n">
-        <v>-4.367</v>
+        <v>-3.489</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.0437</v>
+        <v>0.0304</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0261</v>
+        <v>0.0463</v>
       </c>
     </row>
     <row r="42">
@@ -5041,13 +4677,13 @@
         <v>2021</v>
       </c>
       <c r="B42" t="n">
-        <v>-3.739</v>
+        <v>-3.995</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.1845</v>
+        <v>-0.0997</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.1185</v>
+        <v>-0.0674</v>
       </c>
     </row>
     <row r="43">
@@ -5055,13 +4691,13 @@
         <v>2022</v>
       </c>
       <c r="B43" t="n">
-        <v>0.775</v>
+        <v>-1.557</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1107</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0746</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Cerebro v1.1 — civilizational forecasting engine
Performance:
- Brier 0.1935, ECE 0.0608, Infinity Score all 6 gates green
- 130 tests passing, 86% coverage

Architecture:
- OECD global expansion (6 countries, 41 quality episodes)
- Coupled state vector with shadow validation
- Era-split Gaussian Process sister engine (MAE 1.96)
- Honeycomb ensemble fusion with wide-interval boost
- Quality gate (honey not water principle)
- Pre-sort stratified episode sampling
- Dynamic activation thresholds (coupling >= 60, honeycomb >= 30)
- Live feedback loop for closed window scoring
- Oracle API live on port 5050
- Leading indicators: youth unemployment, enrollment, birth rate

Key fix: wide-interval boost now fires on MIN_TRAIN early return path
ECE 0.0608 — operational weather forecasting tier

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/cerebro_harm_clock_phase1.xlsx
+++ b/cerebro_harm_clock_phase1.xlsx
@@ -111,13 +111,13 @@
     <font>
       <name val="Arial"/>
       <b val="1"/>
-      <color rgb="FFFF6600"/>
+      <color rgb="FF8B0000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
       <b val="1"/>
-      <color rgb="FF8B0000"/>
+      <color rgb="FFFF6600"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -155,12 +155,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF0F0"/>
+        <fgColor rgb="FFFFF8DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF8DC"/>
+        <fgColor rgb="FFFFF0F0"/>
       </patternFill>
     </fill>
   </fills>
@@ -386,12 +386,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'📈 Charts'!$A$2:$A$43</f>
+              <f>'📈 Charts'!$A$2:$A$37</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'📈 Charts'!$B$2:$B$43</f>
+              <f>'📈 Charts'!$B$2:$B$37</f>
             </numRef>
           </val>
         </ser>
@@ -508,12 +508,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'📈 Charts'!$A$2:$A$43</f>
+              <f>'📈 Charts'!$A$2:$A$37</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'📈 Charts'!$C$2:$C$43</f>
+              <f>'📈 Charts'!$C$2:$C$37</f>
             </numRef>
           </val>
         </ser>
@@ -543,12 +543,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'📈 Charts'!$A$2:$A$43</f>
+              <f>'📈 Charts'!$A$2:$A$37</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'📈 Charts'!$D$2:$D$43</f>
+              <f>'📈 Charts'!$D$2:$D$37</f>
             </numRef>
           </val>
         </ser>
@@ -2317,9 +2317,7 @@
       <c r="C67" s="11" t="inlineStr"/>
       <c r="D67" s="11" t="inlineStr"/>
       <c r="E67" s="11" t="inlineStr"/>
-      <c r="F67" s="11" t="n">
-        <v>5.76</v>
-      </c>
+      <c r="F67" s="11" t="inlineStr"/>
       <c r="G67" s="11" t="inlineStr"/>
       <c r="H67" s="11" t="inlineStr"/>
     </row>
@@ -3456,7 +3454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3529,134 +3527,134 @@
     </row>
     <row r="5" ht="28" customHeight="1">
       <c r="B5" s="17" t="n">
-        <v>1979</v>
+        <v>1993</v>
       </c>
       <c r="C5" s="18" t="n">
-        <v>2.83</v>
+        <v>-5.89</v>
       </c>
       <c r="D5" s="18" t="n">
-        <v>-0.0355</v>
+        <v>-0.0018</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>0.0287</v>
+        <v>0.0073</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="19" t="inlineStr">
         <is>
-          <t>MODERATE SADDLE</t>
+          <t>STRONG SADDLE ⚡</t>
         </is>
       </c>
       <c r="H5" s="20" t="inlineStr">
         <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
         </is>
       </c>
     </row>
     <row r="6" ht="28" customHeight="1">
       <c r="B6" s="17" t="n">
-        <v>1980</v>
+        <v>1994</v>
       </c>
       <c r="C6" s="18" t="n">
-        <v>3.04</v>
+        <v>-5.89</v>
       </c>
       <c r="D6" s="18" t="n">
-        <v>-0.0405</v>
+        <v>-0.0142</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>0.0098</v>
+        <v>0.0005</v>
       </c>
       <c r="F6" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="19" t="inlineStr">
+        <is>
+          <t>STRONG SADDLE ⚡</t>
+        </is>
+      </c>
+      <c r="H6" s="20" t="inlineStr">
+        <is>
+          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="28" customHeight="1">
+      <c r="B7" s="21" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C7" s="22" t="n">
+        <v>-5.92</v>
+      </c>
+      <c r="D7" s="22" t="n">
+        <v>0.0341</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>0.0312</v>
+      </c>
+      <c r="F7" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="19" t="inlineStr">
+      <c r="G7" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H6" s="20" t="inlineStr">
+      <c r="H7" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="28" customHeight="1">
-      <c r="B7" s="17" t="n">
-        <v>1982</v>
-      </c>
-      <c r="C7" s="18" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="D7" s="18" t="n">
-        <v>-0.022</v>
-      </c>
-      <c r="E7" s="18" t="n">
-        <v>0.0201</v>
-      </c>
-      <c r="F7" s="18" t="n">
+    <row r="8" ht="28" customHeight="1">
+      <c r="B8" s="21" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="22" t="n">
+        <v>-1.64</v>
+      </c>
+      <c r="D8" s="22" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="E8" s="22" t="n">
+        <v>0.0227</v>
+      </c>
+      <c r="F8" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="19" t="inlineStr">
+      <c r="G8" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H7" s="20" t="inlineStr">
+      <c r="H8" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="28" customHeight="1">
-      <c r="B8" s="17" t="n">
-        <v>1985</v>
-      </c>
-      <c r="C8" s="18" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="D8" s="18" t="n">
-        <v>-0.0001</v>
-      </c>
-      <c r="E8" s="18" t="n">
-        <v>0.0135</v>
-      </c>
-      <c r="F8" s="18" t="n">
+    <row r="9" ht="28" customHeight="1">
+      <c r="B9" s="21" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C9" s="22" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="D9" s="22" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>0.0102</v>
+      </c>
+      <c r="F9" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="19" t="inlineStr">
+      <c r="G9" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H8" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="28" customHeight="1">
-      <c r="B9" s="17" t="n">
-        <v>1986</v>
-      </c>
-      <c r="C9" s="18" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="D9" s="18" t="n">
-        <v>-0.0024</v>
-      </c>
-      <c r="E9" s="18" t="n">
-        <v>0.0065</v>
-      </c>
-      <c r="F9" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H9" s="20" t="inlineStr">
+      <c r="H9" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
@@ -3664,404 +3662,269 @@
     </row>
     <row r="10" ht="28" customHeight="1">
       <c r="B10" s="21" t="n">
-        <v>1993</v>
+        <v>2004</v>
       </c>
       <c r="C10" s="22" t="n">
-        <v>-2.22</v>
+        <v>-2.5</v>
       </c>
       <c r="D10" s="22" t="n">
-        <v>-0.0575</v>
+        <v>0.0115</v>
       </c>
       <c r="E10" s="22" t="n">
-        <v>0.0115</v>
+        <v>0.0081</v>
       </c>
       <c r="F10" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="23" t="inlineStr">
         <is>
-          <t>STRONG SADDLE ⚡</t>
+          <t>MODERATE SADDLE</t>
         </is>
       </c>
       <c r="H10" s="24" t="inlineStr">
         <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="11" ht="28" customHeight="1">
       <c r="B11" s="21" t="n">
-        <v>1995</v>
+        <v>2006</v>
       </c>
       <c r="C11" s="22" t="n">
-        <v>-3.36</v>
+        <v>-2.31</v>
       </c>
       <c r="D11" s="22" t="n">
-        <v>-0.0491</v>
+        <v>0.0743</v>
       </c>
       <c r="E11" s="22" t="n">
-        <v>0.0102</v>
+        <v>0.0569</v>
       </c>
       <c r="F11" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="23" t="inlineStr">
         <is>
-          <t>STRONG SADDLE ⚡</t>
+          <t>MODERATE SADDLE</t>
         </is>
       </c>
       <c r="H11" s="24" t="inlineStr">
         <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="12" ht="28" customHeight="1">
       <c r="B12" s="21" t="n">
-        <v>1996</v>
+        <v>2008</v>
       </c>
       <c r="C12" s="22" t="n">
-        <v>-2.23</v>
+        <v>-2.72</v>
       </c>
       <c r="D12" s="22" t="n">
-        <v>-0.0003</v>
+        <v>0.0589</v>
       </c>
       <c r="E12" s="22" t="n">
-        <v>0.0191</v>
+        <v>0.0394</v>
       </c>
       <c r="F12" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="23" t="inlineStr">
         <is>
-          <t>STRONG SADDLE ⚡</t>
+          <t>MODERATE SADDLE</t>
         </is>
       </c>
       <c r="H12" s="24" t="inlineStr">
         <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="13" ht="28" customHeight="1">
       <c r="B13" s="21" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
       <c r="C13" s="22" t="n">
-        <v>-2.97</v>
+        <v>-2.72</v>
       </c>
       <c r="D13" s="22" t="n">
-        <v>-0.0041</v>
+        <v>0.0614</v>
       </c>
       <c r="E13" s="22" t="n">
-        <v>0.0221</v>
+        <v>0.0434</v>
       </c>
       <c r="F13" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="23" t="inlineStr">
         <is>
-          <t>STRONG SADDLE ⚡</t>
+          <t>MODERATE SADDLE</t>
         </is>
       </c>
       <c r="H13" s="24" t="inlineStr">
         <is>
-          <t>⚡ STRONG SIGNAL: Maximum momentum loading detected. Clock still moving negative but deceleration confirmed. Check leading indicators now — reversal pressure building.</t>
+          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="14" ht="28" customHeight="1">
-      <c r="B14" s="17" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C14" s="18" t="n">
-        <v>-1.49</v>
-      </c>
-      <c r="D14" s="18" t="n">
-        <v>0.0494</v>
-      </c>
-      <c r="E14" s="18" t="n">
-        <v>0.0179</v>
-      </c>
-      <c r="F14" s="18" t="n">
+      <c r="B14" s="21" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C14" s="22" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D14" s="22" t="n">
+        <v>0.1243</v>
+      </c>
+      <c r="E14" s="22" t="n">
+        <v>0.0795</v>
+      </c>
+      <c r="F14" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="19" t="inlineStr">
+      <c r="G14" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H14" s="20" t="inlineStr">
+      <c r="H14" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="15" ht="28" customHeight="1">
-      <c r="B15" s="17" t="n">
-        <v>2002</v>
-      </c>
-      <c r="C15" s="18" t="n">
-        <v>-1.54</v>
-      </c>
-      <c r="D15" s="18" t="n">
-        <v>0.0351</v>
-      </c>
-      <c r="E15" s="18" t="n">
-        <v>0.0158</v>
-      </c>
-      <c r="F15" s="18" t="n">
+      <c r="B15" s="21" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C15" s="22" t="n">
+        <v>-1.12</v>
+      </c>
+      <c r="D15" s="22" t="n">
+        <v>0.1391</v>
+      </c>
+      <c r="E15" s="22" t="n">
+        <v>0.07489999999999999</v>
+      </c>
+      <c r="F15" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="19" t="inlineStr">
+      <c r="G15" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H15" s="20" t="inlineStr">
+      <c r="H15" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="16" ht="28" customHeight="1">
-      <c r="B16" s="17" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C16" s="18" t="n">
-        <v>-2.42</v>
-      </c>
-      <c r="D16" s="18" t="n">
-        <v>0.0164</v>
-      </c>
-      <c r="E16" s="18" t="n">
-        <v>0.0213</v>
-      </c>
-      <c r="F16" s="18" t="n">
+      <c r="B16" s="21" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="22" t="n">
+        <v>-0.79</v>
+      </c>
+      <c r="D16" s="22" t="n">
+        <v>0.1216</v>
+      </c>
+      <c r="E16" s="22" t="n">
+        <v>0.0596</v>
+      </c>
+      <c r="F16" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G16" s="19" t="inlineStr">
+      <c r="G16" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H16" s="20" t="inlineStr">
+      <c r="H16" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="17" ht="28" customHeight="1">
-      <c r="B17" s="17" t="n">
-        <v>2008</v>
-      </c>
-      <c r="C17" s="18" t="n">
-        <v>-2.35</v>
-      </c>
-      <c r="D17" s="18" t="n">
-        <v>0.0392</v>
-      </c>
-      <c r="E17" s="18" t="n">
-        <v>0.0352</v>
-      </c>
-      <c r="F17" s="18" t="n">
+      <c r="B17" s="21" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C17" s="22" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D17" s="22" t="n">
+        <v>0.1342</v>
+      </c>
+      <c r="E17" s="22" t="n">
+        <v>0.06660000000000001</v>
+      </c>
+      <c r="F17" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="19" t="inlineStr">
+      <c r="G17" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H17" s="20" t="inlineStr">
+      <c r="H17" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="18" ht="28" customHeight="1">
-      <c r="B18" s="17" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C18" s="18" t="n">
-        <v>-1.98</v>
-      </c>
-      <c r="D18" s="18" t="n">
-        <v>0.0774</v>
-      </c>
-      <c r="E18" s="18" t="n">
-        <v>0.0551</v>
-      </c>
-      <c r="F18" s="18" t="n">
+      <c r="B18" s="21" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="22" t="n">
+        <v>-3.08</v>
+      </c>
+      <c r="D18" s="22" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="E18" s="22" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="F18" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="19" t="inlineStr">
+      <c r="G18" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H18" s="20" t="inlineStr">
+      <c r="H18" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
       </c>
     </row>
     <row r="19" ht="28" customHeight="1">
-      <c r="B19" s="17" t="n">
-        <v>2012</v>
-      </c>
-      <c r="C19" s="18" t="n">
-        <v>-1.52</v>
-      </c>
-      <c r="D19" s="18" t="n">
-        <v>0.0963</v>
-      </c>
-      <c r="E19" s="18" t="n">
-        <v>0.0542</v>
-      </c>
-      <c r="F19" s="18" t="n">
+      <c r="B19" s="21" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C19" s="22" t="n">
+        <v>-0.61</v>
+      </c>
+      <c r="D19" s="22" t="n">
+        <v>0.06569999999999999</v>
+      </c>
+      <c r="E19" s="22" t="n">
+        <v>0.0454</v>
+      </c>
+      <c r="F19" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="19" t="inlineStr">
+      <c r="G19" s="23" t="inlineStr">
         <is>
           <t>MODERATE SADDLE</t>
         </is>
       </c>
-      <c r="H19" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="28" customHeight="1">
-      <c r="B20" s="17" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C20" s="18" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="D20" s="18" t="n">
-        <v>0.107</v>
-      </c>
-      <c r="E20" s="18" t="n">
-        <v>0.0579</v>
-      </c>
-      <c r="F20" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H20" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="28" customHeight="1">
-      <c r="B21" s="17" t="n">
-        <v>2016</v>
-      </c>
-      <c r="C21" s="18" t="n">
-        <v>-1.69</v>
-      </c>
-      <c r="D21" s="18" t="n">
-        <v>0.0683</v>
-      </c>
-      <c r="E21" s="18" t="n">
-        <v>0.0424</v>
-      </c>
-      <c r="F21" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H21" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="28" customHeight="1">
-      <c r="B22" s="17" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C22" s="18" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D22" s="18" t="n">
-        <v>0.1026</v>
-      </c>
-      <c r="E22" s="18" t="n">
-        <v>0.06270000000000001</v>
-      </c>
-      <c r="F22" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H22" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="28" customHeight="1">
-      <c r="B23" s="17" t="n">
-        <v>2020</v>
-      </c>
-      <c r="C23" s="18" t="n">
-        <v>-3.49</v>
-      </c>
-      <c r="D23" s="18" t="n">
-        <v>0.0304</v>
-      </c>
-      <c r="E23" s="18" t="n">
-        <v>0.0463</v>
-      </c>
-      <c r="F23" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G23" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H23" s="20" t="inlineStr">
-        <is>
-          <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="28" customHeight="1">
-      <c r="B24" s="17" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C24" s="18" t="n">
-        <v>-1.56</v>
-      </c>
-      <c r="D24" s="18" t="n">
-        <v>0.07729999999999999</v>
-      </c>
-      <c r="E24" s="18" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F24" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="19" t="inlineStr">
-        <is>
-          <t>MODERATE SADDLE</t>
-        </is>
-      </c>
-      <c r="H24" s="20" t="inlineStr">
+      <c r="H19" s="24" t="inlineStr">
         <is>
           <t>Moderate inflection signal. Velocity negative, acceleration positive. Monitor for confirmation.</t>
         </is>
@@ -4082,7 +3945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4114,590 +3977,506 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1979</v>
+        <v>1987</v>
       </c>
       <c r="B2" t="n">
-        <v>2.83</v>
+        <v>-5.121</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0355</v>
+        <v>-0.013</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0287</v>
+        <v>-0.0317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1980</v>
+        <v>1988</v>
       </c>
       <c r="B3" t="n">
-        <v>3.041</v>
+        <v>-4.997</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0405</v>
+        <v>0.0028</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0098</v>
+        <v>-0.0251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1982</v>
+        <v>1989</v>
       </c>
       <c r="B4" t="n">
-        <v>2.55</v>
+        <v>-5.15</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.022</v>
+        <v>0.0003</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0201</v>
+        <v>-0.0066</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1984</v>
+        <v>1990</v>
       </c>
       <c r="B5" t="n">
-        <v>3.571</v>
+        <v>-5.834</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0247</v>
+        <v>-0.0237</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0201</v>
+        <v>-0.0036</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1985</v>
+        <v>1991</v>
       </c>
       <c r="B6" t="n">
-        <v>3.037</v>
+        <v>-5.469</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0001</v>
+        <v>-0.0157</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0135</v>
+        <v>-0.0062</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1986</v>
+        <v>1992</v>
       </c>
       <c r="B7" t="n">
-        <v>2.477</v>
+        <v>-6.94</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0024</v>
+        <v>-0.0597</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0065</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="B8" t="n">
-        <v>2.266</v>
+        <v>-5.889</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0435</v>
+        <v>-0.0018</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0227</v>
+        <v>0.0073</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1988</v>
+        <v>1994</v>
       </c>
       <c r="B9" t="n">
-        <v>1.269</v>
+        <v>-5.893</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0589</v>
+        <v>-0.0142</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0196</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1989</v>
+        <v>1995</v>
       </c>
       <c r="B10" t="n">
-        <v>0.503</v>
+        <v>-5.918</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0658</v>
+        <v>0.0341</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0211</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1990</v>
+        <v>1996</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.491</v>
+        <v>-3.858</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0919</v>
+        <v>0.0677</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0161</v>
+        <v>0.0232</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1991</v>
+        <v>1997</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.737</v>
+        <v>-4.789</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0669</v>
+        <v>0.0368</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0026</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1992</v>
+        <v>1998</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.89</v>
+        <v>-2.465</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0798</v>
+        <v>0.1151</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.0047</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1993</v>
+        <v>1999</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.216</v>
+        <v>-3.741</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0575</v>
+        <v>0.0039</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0115</v>
+        <v>-0.0213</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1994</v>
+        <v>2000</v>
       </c>
       <c r="B15" t="n">
-        <v>-2.846</v>
+        <v>-1.639</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.0703</v>
+        <v>0.105</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0011</v>
+        <v>0.0227</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1995</v>
+        <v>2001</v>
       </c>
       <c r="B16" t="n">
-        <v>-3.363</v>
+        <v>-2.847</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0491</v>
+        <v>-0.0127</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0102</v>
+        <v>-0.0426</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1996</v>
+        <v>2002</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.226</v>
+        <v>-2.703</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.0003</v>
+        <v>0.0346</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0191</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1997</v>
+        <v>2003</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.97</v>
+        <v>-4.536</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.0041</v>
+        <v>-0.09660000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0221</v>
+        <v>-0.0672</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1998</v>
+        <v>2004</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.915</v>
+        <v>-2.502</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0483</v>
+        <v>0.0115</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0325</v>
+        <v>0.0081</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1999</v>
+        <v>2005</v>
       </c>
       <c r="B20" t="n">
-        <v>-2.594</v>
+        <v>-4.486</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.0123</v>
+        <v>-0.0594</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.004</v>
+        <v>-0.0313</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.486</v>
+        <v>-2.307</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0494</v>
+        <v>0.0743</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0179</v>
+        <v>0.0569</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2001</v>
+        <v>2007</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.498</v>
+        <v>-4.564</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0139</v>
+        <v>-0.0687</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0115</v>
+        <v>-0.0267</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2002</v>
+        <v>2008</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.542</v>
+        <v>-2.72</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0351</v>
+        <v>0.0589</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0158</v>
+        <v>0.0394</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2003</v>
+        <v>2009</v>
       </c>
       <c r="B24" t="n">
-        <v>-2.91</v>
+        <v>-5.728</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.0475</v>
+        <v>-0.114</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0323</v>
+        <v>-0.06279999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="B25" t="n">
-        <v>-1.66</v>
+        <v>-2.724</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.0054</v>
+        <v>0.0614</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.0064</v>
+        <v>0.0434</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="B26" t="n">
-        <v>-3.53</v>
+        <v>-5.289</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.0663</v>
+        <v>-0.0856</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.0338</v>
+        <v>-0.0482</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B27" t="n">
-        <v>-2.417</v>
+        <v>-1.998</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0164</v>
+        <v>0.1243</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0213</v>
+        <v>0.0795</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="B28" t="n">
-        <v>-4.3</v>
+        <v>-4.435</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.08799999999999999</v>
+        <v>-0.0571</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0275</v>
+        <v>-0.0395</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.354</v>
+        <v>-1.115</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0392</v>
+        <v>0.1391</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0352</v>
+        <v>0.07489999999999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="B30" t="n">
-        <v>-4.403</v>
+        <v>-3.965</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.06619999999999999</v>
+        <v>-0.06560000000000001</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0275</v>
+        <v>-0.0633</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.977</v>
+        <v>-0.787</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0774</v>
+        <v>0.1216</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0551</v>
+        <v>0.0596</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="B32" t="n">
-        <v>-4.356</v>
+        <v>-3.367</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.0667</v>
+        <v>-0.075</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0353</v>
+        <v>-0.07140000000000001</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="B33" t="n">
-        <v>-1.515</v>
+        <v>0.06</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0963</v>
+        <v>0.1342</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0542</v>
+        <v>0.06660000000000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="B34" t="n">
-        <v>-3.745</v>
+        <v>-2.901</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.0589</v>
+        <v>-0.07049999999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0455</v>
+        <v>-0.064</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="B35" t="n">
-        <v>-1.148</v>
+        <v>-3.077</v>
       </c>
       <c r="C35" t="n">
-        <v>0.107</v>
+        <v>0.0097</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0579</v>
+        <v>0.0282</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="B36" t="n">
-        <v>-4.083</v>
+        <v>-2.732</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.0856</v>
+        <v>-0.0718</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.0606</v>
+        <v>-0.0687</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.695</v>
+        <v>-0.607</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0683</v>
+        <v>0.06569999999999999</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0424</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B38" t="n">
-        <v>-4.401</v>
-      </c>
-      <c r="C38" t="n">
-        <v>-0.1084</v>
-      </c>
-      <c r="D38" t="n">
-        <v>-0.0718</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B39" t="n">
-        <v>-1.005</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.1026</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.06270000000000001</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B40" t="n">
-        <v>-3.877</v>
-      </c>
-      <c r="C40" t="n">
-        <v>-0.0727</v>
-      </c>
-      <c r="D40" t="n">
-        <v>-0.047</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B41" t="n">
-        <v>-3.489</v>
-      </c>
-      <c r="C41" t="n">
-        <v>0.0304</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.0463</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B42" t="n">
-        <v>-3.995</v>
-      </c>
-      <c r="C42" t="n">
-        <v>-0.0997</v>
-      </c>
-      <c r="D42" t="n">
-        <v>-0.0674</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B43" t="n">
-        <v>-1.557</v>
-      </c>
-      <c r="C43" t="n">
-        <v>0.07729999999999999</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0.05</v>
+        <v>0.0454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>